<commit_message>
added some extra commandline options
</commit_message>
<xml_diff>
--- a/resources/Formulas.xlsx
+++ b/resources/Formulas.xlsx
@@ -14,25 +14,55 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>A</t>
   </si>
   <si>
     <t>B</t>
+  </si>
+  <si>
+    <t>é</t>
+  </si>
+  <si>
+    <t>ñ</t>
+  </si>
+  <si>
+    <t>Σ</t>
+  </si>
+  <si>
+    <t>Chars</t>
+  </si>
+  <si>
+    <t>Chars comment</t>
+  </si>
+  <si>
+    <t>Greek Capital Letter Sigma cannot be encoded in latin-1</t>
+  </si>
+  <si>
+    <t>Latin small letter e with acute</t>
+  </si>
+  <si>
+    <t>&amp;#233;</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Verdana"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -55,8 +85,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -361,26 +392,33 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="51.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -388,8 +426,17 @@
         <f>A2*2</f>
         <v>2</v>
       </c>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -397,8 +444,11 @@
         <f t="shared" ref="B3:B4" si="0">A3*2</f>
         <v>4</v>
       </c>
+      <c r="C3" t="s">
+        <v>3</v>
+      </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -406,8 +456,21 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
+      <c r="C4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <f>SUM(B2:B4)</f>
+        <v>12</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>